<commit_message>
2020 HIVE system update, yury 20201224
</commit_message>
<xml_diff>
--- a/src/main/webapp/uploadFiles/file/Fund_Raise_Info.xlsx
+++ b/src/main/webapp/uploadFiles/file/Fund_Raise_Info.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liuzengzhen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VG967GM\Documents\Adocument\EY\2020MID\TINA修改需求\导入表模板修改和新增\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0E13BB-300F-4A30-AFEA-8F9BCCCB1BD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9765"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DETAIL" sheetId="2" r:id="rId1"/>
+    <sheet name="本表新基金需填列" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,11 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>基金ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>FUND_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,6 +35,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>F100066-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>AMOUNT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -46,34 +47,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>份额</t>
+    <t>F100096-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>金额</t>
+    <t>LEVEL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>分级基金代码（非真分级可留空）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F002957-01</t>
-  </si>
-  <si>
-    <t>002957</t>
-  </si>
-  <si>
-    <t>LEVEL</t>
+    <t>基金ID</t>
+  </si>
+  <si>
+    <t>分级基金代码
+（非真分级基金不需要填）</t>
+  </si>
+  <si>
+    <t>设立时募集基金份额</t>
+  </si>
+  <si>
+    <t>分级简称
+（如，A/B级，C级，非真分级基金不需要填）</t>
   </si>
   <si>
     <t>A级</t>
+  </si>
+  <si>
+    <t>B级</t>
+  </si>
+  <si>
+    <t>设立时募集金额
+（含本息，元）</t>
+  </si>
+  <si>
+    <t>示例，填完请删除</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt; Text &gt;</t>
+  </si>
+  <si>
+    <t>&lt; Accounting &gt;</t>
+  </si>
+  <si>
+    <t>AMOUNT_PRINCIPAL</t>
+  </si>
+  <si>
+    <t>AMOUNT_INTEREST</t>
+  </si>
+  <si>
+    <t>设立时募集金额-本金</t>
+  </si>
+  <si>
+    <t>设立时募集金额-利息</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -92,19 +122,37 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10.5"/>
       <color theme="1"/>
       <name val="黑体"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,34 +164,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -159,7 +230,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -420,72 +491,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="21.44140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
+      <c r="B4" s="1">
+        <v>100066</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>703810487.46000004</v>
+      </c>
+      <c r="E4" s="2">
+        <v>703810487.46000004</v>
+      </c>
+      <c r="F4" s="2">
+        <v>703810487.46000004</v>
+      </c>
+      <c r="G4" s="2">
+        <v>703810487.46000004</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100067</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="E5" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="F5" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="G5" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1186753840.53</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1186753840.53</v>
-      </c>
+      <c r="D6" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="E6" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="F6" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="G6" s="2">
+        <v>775135275.30999994</v>
+      </c>
+      <c r="H6" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H4:H6"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>